<commit_message>
More data and IDA
</commit_message>
<xml_diff>
--- a/Assignment3/MatrixMultiplication/DataMM.xlsx
+++ b/Assignment3/MatrixMultiplication/DataMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitrihooftman/Desktop/PerformanceEngineering/performance-engineering/Assignment3/MatrixMultiplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978F3EB7-CA4C-1F46-B2E4-723E01742155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A7C26D-EFC7-E64B-96EF-5C109FB33C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3720" windowWidth="38400" windowHeight="21100" xr2:uid="{5A3C439C-579D-0240-9745-8FE294455EA8}"/>
   </bookViews>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F331EBB-3658-5B47-9DDA-F500350F20CC}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +650,7 @@
         <v>505408</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H10" si="0">ROUND(((F4 - G4) / F4) * 100, 0)</f>
+        <f t="shared" ref="H4:H22" si="0">ROUND(((F4 - G4) / F4) * 100, 0)</f>
         <v>86</v>
       </c>
       <c r="I4" s="2">
@@ -838,6 +838,366 @@
       </c>
       <c r="L10" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>461</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>23837684</v>
+      </c>
+      <c r="E11">
+        <v>25093083</v>
+      </c>
+      <c r="F11">
+        <v>28747</v>
+      </c>
+      <c r="G11">
+        <v>14260</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="2">
+        <v>13678482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>439</v>
+      </c>
+      <c r="C12">
+        <v>612</v>
+      </c>
+      <c r="D12">
+        <v>1132344495</v>
+      </c>
+      <c r="E12">
+        <v>610098078</v>
+      </c>
+      <c r="F12">
+        <v>301008</v>
+      </c>
+      <c r="G12">
+        <v>71408</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="I12" s="2">
+        <v>399326069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>460</v>
+      </c>
+      <c r="B13">
+        <v>689</v>
+      </c>
+      <c r="C13">
+        <v>809</v>
+      </c>
+      <c r="D13">
+        <v>8093239977</v>
+      </c>
+      <c r="E13">
+        <v>3391057734</v>
+      </c>
+      <c r="F13">
+        <v>3005137</v>
+      </c>
+      <c r="G13">
+        <v>621630</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1826409408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>873</v>
+      </c>
+      <c r="B14">
+        <v>987</v>
+      </c>
+      <c r="C14">
+        <v>611</v>
+      </c>
+      <c r="D14">
+        <v>16537254902</v>
+      </c>
+      <c r="E14">
+        <v>6606571601</v>
+      </c>
+      <c r="F14">
+        <v>6412068</v>
+      </c>
+      <c r="G14">
+        <v>1179174</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3153030696</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>263</v>
+      </c>
+      <c r="B15">
+        <v>542</v>
+      </c>
+      <c r="C15">
+        <v>682</v>
+      </c>
+      <c r="D15">
+        <v>3101765457</v>
+      </c>
+      <c r="E15">
+        <v>1329933418</v>
+      </c>
+      <c r="F15">
+        <v>893578</v>
+      </c>
+      <c r="G15">
+        <v>44167</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="I15" s="2">
+        <v>850191702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>836</v>
+      </c>
+      <c r="C16">
+        <v>710</v>
+      </c>
+      <c r="D16">
+        <v>935857312</v>
+      </c>
+      <c r="E16">
+        <v>474943232</v>
+      </c>
+      <c r="F16">
+        <v>344619</v>
+      </c>
+      <c r="G16">
+        <v>122864</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I16" s="2">
+        <v>303112921</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>992</v>
+      </c>
+      <c r="B17">
+        <v>403</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>242708708</v>
+      </c>
+      <c r="E17">
+        <v>160322043</v>
+      </c>
+      <c r="F17">
+        <v>31848</v>
+      </c>
+      <c r="G17">
+        <v>16287</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="I17" s="2">
+        <v>101737111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>733</v>
+      </c>
+      <c r="B18">
+        <v>339</v>
+      </c>
+      <c r="C18">
+        <v>385</v>
+      </c>
+      <c r="D18">
+        <v>3051855365</v>
+      </c>
+      <c r="E18">
+        <v>1353288115</v>
+      </c>
+      <c r="F18">
+        <v>588402</v>
+      </c>
+      <c r="G18">
+        <v>66978</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="I18" s="2">
+        <v>711956200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>973</v>
+      </c>
+      <c r="B19">
+        <v>97</v>
+      </c>
+      <c r="C19">
+        <v>942</v>
+      </c>
+      <c r="D19">
+        <v>2851377745</v>
+      </c>
+      <c r="E19">
+        <v>1188223003</v>
+      </c>
+      <c r="F19">
+        <v>542545</v>
+      </c>
+      <c r="G19">
+        <v>100067</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="I19" s="2">
+        <v>773122899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>654</v>
+      </c>
+      <c r="B20">
+        <v>959</v>
+      </c>
+      <c r="C20">
+        <v>638</v>
+      </c>
+      <c r="D20">
+        <v>12589054691</v>
+      </c>
+      <c r="E20">
+        <v>5471941717</v>
+      </c>
+      <c r="F20">
+        <v>4843469</v>
+      </c>
+      <c r="G20">
+        <v>786366</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2593891840</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>47</v>
+      </c>
+      <c r="B21">
+        <v>182</v>
+      </c>
+      <c r="C21">
+        <v>700</v>
+      </c>
+      <c r="D21">
+        <v>221359403</v>
+      </c>
+      <c r="E21">
+        <v>140658675</v>
+      </c>
+      <c r="F21">
+        <v>64140</v>
+      </c>
+      <c r="G21">
+        <v>23956</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I21" s="2">
+        <v>97192970</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>791</v>
+      </c>
+      <c r="B22">
+        <v>197</v>
+      </c>
+      <c r="C22">
+        <v>434</v>
+      </c>
+      <c r="D22">
+        <v>2166540466</v>
+      </c>
+      <c r="E22">
+        <v>1072472631</v>
+      </c>
+      <c r="F22">
+        <v>338962</v>
+      </c>
+      <c r="G22">
+        <v>63584</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="I22" s="2">
+        <v>689245593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>